<commit_message>
lab updates - still in progress
</commit_message>
<xml_diff>
--- a/labs/sample-adusers.xlsx
+++ b/labs/sample-adusers.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds0934\Google Drive\PCM\Customers\MetLife\SCRIPTS\ImportUsers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ActiveDirectory\labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F07A5EA-287C-4BE5-8DC2-ABE248087341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="31935" yWindow="2430" windowWidth="24555" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="11" r:id="rId1"/>
@@ -47,22 +48,33 @@
     <definedName name="Managers">Managers!$A$2:$B$10</definedName>
     <definedName name="msExch1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>David Stein</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -158,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -206,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -230,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -254,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -278,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -302,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -326,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -350,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -374,7 +386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -398,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -422,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -446,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -470,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -494,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -518,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -542,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -566,7 +578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -590,7 +602,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -614,7 +626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -638,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -662,7 +674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -686,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -710,7 +722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -734,7 +746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -758,7 +770,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -782,7 +794,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -806,7 +818,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -830,7 +842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -854,7 +866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0">
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -878,7 +890,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -902,7 +914,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -926,7 +938,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -950,7 +962,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -974,7 +986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -998,7 +1010,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0">
+    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -1022,7 +1034,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -1046,7 +1058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0" shapeId="0">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -1070,7 +1082,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0" shapeId="0">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -1094,7 +1106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0">
+    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -1118,7 +1130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -1143,7 +1155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -1167,7 +1179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -1191,7 +1203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0">
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
       <text>
         <r>
           <rPr>
@@ -1215,7 +1227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
       <text>
         <r>
           <rPr>
@@ -1239,7 +1251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
       <text>
         <r>
           <rPr>
@@ -1268,12 +1280,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>David Stein</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1297,7 +1309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1844,7 +1856,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -1934,16 +1946,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1956,45 +1960,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2039,7 +2033,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2351,2712 +2345,2688 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31" style="11" customWidth="1"/>
-    <col min="17" max="17" width="32.42578125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.28515625" customWidth="1"/>
-    <col min="25" max="25" width="46" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="34" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="30" style="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="48.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="43" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="43" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="44" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="24.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="48" max="50" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="33.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="58.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="7" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:52" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AK1" s="16" t="s">
+      <c r="AK1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AR1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AU1" s="18" t="s">
+      <c r="AU1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AV1" s="18" t="s">
+      <c r="AV1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="10" t="s">
+      <c r="AW1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="18" t="s">
+      <c r="AX1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="10" t="s">
+      <c r="AY1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AZ1" s="10" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="10">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <v>123123</v>
       </c>
-      <c r="F2" s="2" t="str">
+      <c r="F2" s="11" t="str">
         <f t="shared" ref="F2:F20" si="0">CONCATENATE("CN=",H2,",",G2)</f>
         <v>CN=rmoritz,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="N2" s="24" t="str">
-        <f>TEXT(D2,"0000000")</f>
+      <c r="N2" s="10" t="str">
+        <f t="shared" ref="N2:N20" si="1">TEXT(D2,"0000000")</f>
         <v>0123123</v>
       </c>
-      <c r="O2" t="str">
-        <f t="shared" ref="O2:O20" si="1">CONCATENATE(M2,", ",K2)</f>
+      <c r="O2" s="11" t="str">
+        <f t="shared" ref="O2:O20" si="2">CONCATENATE(M2,", ",K2)</f>
         <v>Smith, John</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="11" t="str">
+      <c r="Y2" s="13" t="str">
         <f>CONCATENATE($H2,"@",$C2)</f>
         <v>rmoritz@contoso.com</v>
       </c>
-      <c r="Z2" s="13" t="str">
-        <f t="shared" ref="Z2:Z20" si="2">H2</f>
+      <c r="Z2" s="10" t="str">
+        <f t="shared" ref="Z2:Z20" si="3">H2</f>
         <v>rmoritz</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="11">
         <v>10004</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK2" s="17">
+      <c r="AK2" s="15">
         <v>23452</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AL2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="11" t="str">
-        <f t="shared" ref="AQ2:AQ20" si="3">Y2</f>
+      <c r="AQ2" s="13" t="str">
+        <f t="shared" ref="AQ2:AQ20" si="4">Y2</f>
         <v>rmoritz@contoso.com</v>
       </c>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" t="str">
-        <f>IF(ISERROR(VLOOKUP(D2,JournalArray2,5,FALSE)),"",VLOOKUP(D2,JournalArray2,5,FALSE))</f>
+      <c r="AS2" s="17"/>
+      <c r="AT2" s="11" t="str">
+        <f t="shared" ref="AT2:AT20" si="5">IF(ISERROR(VLOOKUP(D2,JournalArray2,5,FALSE)),"",VLOOKUP(D2,JournalArray2,5,FALSE))</f>
         <v/>
       </c>
-      <c r="AU2" s="11" t="str">
+      <c r="AU2" s="13" t="str">
         <f>IF(OR(AT2="INCLUDE",AT2="ONHOLD"),CONCATENATE("skype:",AQ2),"")</f>
         <v/>
       </c>
-      <c r="AV2" s="6" t="str">
-        <f t="shared" ref="AV2:AV20" si="4">Y2</f>
+      <c r="AV2" s="13" t="str">
+        <f t="shared" ref="AV2:AV20" si="6">Y2</f>
         <v>rmoritz@contoso.com</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AW2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX2" s="6" t="str">
-        <f t="shared" ref="AX2:AX20" si="5">Y2</f>
+      <c r="AX2" s="13" t="str">
+        <f t="shared" ref="AX2:AX20" si="7">Y2</f>
         <v>rmoritz@contoso.com</v>
       </c>
-      <c r="AY2" t="str">
-        <f t="shared" ref="AY2:AY20" si="6">CONCATENATE("SIP:",Y2)</f>
+      <c r="AY2" s="11" t="str">
+        <f t="shared" ref="AY2:AY20" si="8">CONCATENATE("SIP:",Y2)</f>
         <v>SIP:rmoritz@contoso.com</v>
       </c>
-      <c r="AZ2" s="2" t="str">
-        <f t="shared" ref="AZ2:AZ20" si="7">CONCATENATE("SMTP:",Y2,";","SIP:",Y2)</f>
+      <c r="AZ2" s="11" t="str">
+        <f t="shared" ref="AZ2:AZ20" si="9">CONCATENATE("SMTP:",Y2,";","SIP:",Y2)</f>
         <v>SMTP:rmoritz@contoso.com;SIP:rmoritz@contoso.com</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="10">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <v>234234</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="12">
         <v>123123</v>
       </c>
-      <c r="F3" s="2" t="str">
+      <c r="F3" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=dcaccamo,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="N3" s="24" t="str">
-        <f>TEXT(D3,"0000000")</f>
+      <c r="N3" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0234234</v>
       </c>
-      <c r="O3" t="str">
-        <f t="shared" si="1"/>
+      <c r="O3" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Stewart, James</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y3" s="11" t="str">
-        <f t="shared" ref="Y3:Y20" si="8">CONCATENATE($H3,"@",$C3)</f>
+      <c r="Y3" s="13" t="str">
+        <f t="shared" ref="Y3:Y20" si="10">CONCATENATE($H3,"@",$C3)</f>
         <v>dcaccamo@contoso.com</v>
       </c>
-      <c r="Z3" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z3" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>dcaccamo</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AB3" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="11">
         <v>10004</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK3" s="17">
+      <c r="AK3" s="15">
         <v>23452</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AL3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ3" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>dcaccamo@contoso.com</v>
-      </c>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" t="str">
-        <f>IF(ISERROR(VLOOKUP(D3,JournalArray2,5,FALSE)),"",VLOOKUP(D3,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU3" s="11" t="str">
-        <f t="shared" ref="AU3:AU20" si="9">IF(OR(AT3="INCLUDE",AT3="ONHOLD"),CONCATENATE("skype:",AQ3),"")</f>
-        <v/>
-      </c>
-      <c r="AV3" s="6" t="str">
+      <c r="AQ3" s="13" t="str">
         <f t="shared" si="4"/>
         <v>dcaccamo@contoso.com</v>
       </c>
-      <c r="AW3" s="2" t="s">
+      <c r="AS3" s="17"/>
+      <c r="AT3" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU3" s="13" t="str">
+        <f t="shared" ref="AU3:AU20" si="11">IF(OR(AT3="INCLUDE",AT3="ONHOLD"),CONCATENATE("skype:",AQ3),"")</f>
+        <v/>
+      </c>
+      <c r="AV3" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>dcaccamo@contoso.com</v>
+      </c>
+      <c r="AW3" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX3" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX3" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>dcaccamo@contoso.com</v>
       </c>
-      <c r="AY3" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY3" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:dcaccamo@contoso.com</v>
       </c>
-      <c r="AZ3" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ3" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:dcaccamo@contoso.com;SIP:dcaccamo@contoso.com</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="10">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <v>345345</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="12">
         <v>123123</v>
       </c>
-      <c r="F4" s="2" t="str">
+      <c r="F4" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=lrhoads,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="24" t="str">
-        <f>TEXT(D4,"0000000")</f>
+      <c r="N4" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0345345</v>
       </c>
-      <c r="O4" t="str">
-        <f t="shared" si="1"/>
+      <c r="O4" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Bennett, Jerry</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y4" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y4" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>lrhoads@contoso.com</v>
       </c>
-      <c r="Z4" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z4" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>lrhoads</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AB4" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="11">
         <v>10004</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AH4" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AI4" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AJ4" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK4" s="17">
+      <c r="AK4" s="15">
         <v>23452</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AL4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ4" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>lrhoads@contoso.com</v>
-      </c>
-      <c r="AR4" s="21"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" t="str">
-        <f>IF(ISERROR(VLOOKUP(D4,JournalArray2,5,FALSE)),"",VLOOKUP(D4,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU4" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV4" s="6" t="str">
+      <c r="AQ4" s="13" t="str">
         <f t="shared" si="4"/>
         <v>lrhoads@contoso.com</v>
       </c>
-      <c r="AW4" s="2" t="s">
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU4" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV4" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>lrhoads@contoso.com</v>
+      </c>
+      <c r="AW4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX4" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX4" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>lrhoads@contoso.com</v>
       </c>
-      <c r="AY4" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY4" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:lrhoads@contoso.com</v>
       </c>
-      <c r="AZ4" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ4" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:lrhoads@contoso.com;SIP:lrhoads@contoso.com</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="10">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>456456</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="12">
         <v>123123</v>
       </c>
-      <c r="F5" s="2" t="str">
+      <c r="F5" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=tfoust,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="N5" s="24" t="str">
-        <f>TEXT(D5,"0000000")</f>
+      <c r="N5" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0456456</v>
       </c>
-      <c r="O5" t="str">
-        <f t="shared" si="1"/>
+      <c r="O5" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Johnson, Kevin</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y5" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>tfoust@contoso.com</v>
       </c>
-      <c r="Z5" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z5" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>tfoust</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AB5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AC5" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="11">
         <v>10004</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AF5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AH5" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AI5" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AJ5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK5" s="17">
+      <c r="AK5" s="15">
         <v>23452</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AL5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ5" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>tfoust@contoso.com</v>
-      </c>
-      <c r="AS5" s="1"/>
-      <c r="AT5" t="str">
-        <f>IF(ISERROR(VLOOKUP(D5,JournalArray2,5,FALSE)),"",VLOOKUP(D5,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU5" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV5" s="6" t="str">
+      <c r="AQ5" s="13" t="str">
         <f t="shared" si="4"/>
         <v>tfoust@contoso.com</v>
       </c>
-      <c r="AW5" s="2" t="s">
+      <c r="AS5" s="17"/>
+      <c r="AT5" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU5" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV5" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>tfoust@contoso.com</v>
+      </c>
+      <c r="AW5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX5" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX5" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>tfoust@contoso.com</v>
       </c>
-      <c r="AY5" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY5" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:tfoust@contoso.com</v>
       </c>
-      <c r="AZ5" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ5" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:tfoust@contoso.com;SIP:tfoust@contoso.com</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="10">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <v>345345</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="12">
         <v>123123</v>
       </c>
-      <c r="F6" s="2" t="str">
+      <c r="F6" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=RSemke,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N6" s="24" t="str">
-        <f>TEXT(D6,"0000000")</f>
+      <c r="N6" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0345345</v>
       </c>
-      <c r="O6" t="str">
-        <f t="shared" si="1"/>
+      <c r="O6" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Harrison, Kyle</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="U6" t="s">
+      <c r="U6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y6" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>RSemke@contoso.com</v>
       </c>
-      <c r="Z6" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z6" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>RSemke</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AC6" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="11">
         <v>10004</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AF6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AH6" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AI6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AJ6" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK6" s="17">
+      <c r="AK6" s="15">
         <v>23452</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AL6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ6" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>RSemke@contoso.com</v>
-      </c>
-      <c r="AS6" s="1"/>
-      <c r="AT6" t="str">
-        <f>IF(ISERROR(VLOOKUP(D6,JournalArray2,5,FALSE)),"",VLOOKUP(D6,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU6" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV6" s="6" t="str">
+      <c r="AQ6" s="13" t="str">
         <f t="shared" si="4"/>
         <v>RSemke@contoso.com</v>
       </c>
-      <c r="AW6" s="2" t="s">
+      <c r="AS6" s="17"/>
+      <c r="AT6" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV6" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>RSemke@contoso.com</v>
+      </c>
+      <c r="AW6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX6" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX6" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>RSemke@contoso.com</v>
       </c>
-      <c r="AY6" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY6" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:RSemke@contoso.com</v>
       </c>
-      <c r="AZ6" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ6" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:RSemke@contoso.com;SIP:RSemke@contoso.com</v>
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="10">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>474747</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="12">
         <v>123123</v>
       </c>
-      <c r="F7" s="2" t="str">
+      <c r="F7" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=jreddy,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="N7" s="24" t="str">
-        <f>TEXT(D7,"0000000")</f>
+      <c r="N7" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0474747</v>
       </c>
-      <c r="O7" t="str">
-        <f t="shared" si="1"/>
+      <c r="O7" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>McSweeney, Kim</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="R7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y7" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y7" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>jreddy@contoso.com</v>
       </c>
-      <c r="Z7" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z7" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>jreddy</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AB7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AC7" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="11">
         <v>10005</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AF7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AH7" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AI7" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AJ7" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK7" s="17">
+      <c r="AK7" s="15">
         <v>23452</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AL7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ7" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>jreddy@contoso.com</v>
-      </c>
-      <c r="AS7" s="1"/>
-      <c r="AT7" t="str">
-        <f>IF(ISERROR(VLOOKUP(D7,JournalArray2,5,FALSE)),"",VLOOKUP(D7,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU7" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV7" s="6" t="str">
+      <c r="AQ7" s="13" t="str">
         <f t="shared" si="4"/>
         <v>jreddy@contoso.com</v>
       </c>
-      <c r="AW7" s="2" t="s">
+      <c r="AS7" s="17"/>
+      <c r="AT7" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU7" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV7" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>jreddy@contoso.com</v>
+      </c>
+      <c r="AW7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX7" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX7" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>jreddy@contoso.com</v>
       </c>
-      <c r="AY7" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY7" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:jreddy@contoso.com</v>
       </c>
-      <c r="AZ7" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ7" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:jreddy@contoso.com;SIP:jreddy@contoso.com</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="10">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <v>256262</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="12">
         <v>123123</v>
       </c>
-      <c r="F8" s="2" t="str">
+      <c r="F8" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=srodriguez,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="24" t="str">
-        <f>TEXT(D8,"0000000")</f>
+      <c r="N8" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0256262</v>
       </c>
-      <c r="O8" t="str">
-        <f t="shared" si="1"/>
+      <c r="O8" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Rodriguez, Larry</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="R8" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y8" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y8" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>srodriguez@contoso.com</v>
       </c>
-      <c r="Z8" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z8" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>srodriguez</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AB8" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AC8" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AD8" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="11">
         <v>10005</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AF8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AH8" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AI8" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AJ8" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK8" s="17">
+      <c r="AK8" s="15">
         <v>23452</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AL8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ8" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>srodriguez@contoso.com</v>
-      </c>
-      <c r="AR8" s="21"/>
-      <c r="AS8" s="1"/>
-      <c r="AT8" t="str">
-        <f>IF(ISERROR(VLOOKUP(D8,JournalArray2,5,FALSE)),"",VLOOKUP(D8,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU8" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV8" s="6" t="str">
+      <c r="AQ8" s="13" t="str">
         <f t="shared" si="4"/>
         <v>srodriguez@contoso.com</v>
       </c>
-      <c r="AW8" s="2" t="s">
+      <c r="AS8" s="17"/>
+      <c r="AT8" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU8" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV8" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>srodriguez@contoso.com</v>
+      </c>
+      <c r="AW8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX8" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX8" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>srodriguez@contoso.com</v>
       </c>
-      <c r="AY8" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY8" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:srodriguez@contoso.com</v>
       </c>
-      <c r="AZ8" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ8" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:srodriguez@contoso.com;SIP:srodriguez@contoso.com</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="10">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="11">
         <v>261514</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="12">
         <v>474747</v>
       </c>
-      <c r="F9" s="2" t="str">
+      <c r="F9" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=amsurber,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="N9" s="24" t="str">
-        <f>TEXT(D9,"0000000")</f>
+      <c r="N9" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0261514</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" si="1"/>
+      <c r="O9" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Taylor, Lisa</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="R9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y9" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y9" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>amsurber@contoso.com</v>
       </c>
-      <c r="Z9" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z9" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>amsurber</v>
       </c>
-      <c r="AB9" s="2" t="s">
+      <c r="AB9" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AC9" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="11">
         <v>10005</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AF9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AH9" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AI9" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AJ9" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK9" s="17">
+      <c r="AK9" s="15">
         <v>23452</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AL9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ9" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>amsurber@contoso.com</v>
-      </c>
-      <c r="AR9" s="21"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" t="str">
-        <f>IF(ISERROR(VLOOKUP(D9,JournalArray2,5,FALSE)),"",VLOOKUP(D9,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU9" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV9" s="6" t="str">
+      <c r="AQ9" s="13" t="str">
         <f t="shared" si="4"/>
         <v>amsurber@contoso.com</v>
       </c>
-      <c r="AW9" s="2" t="s">
+      <c r="AS9" s="17"/>
+      <c r="AT9" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU9" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV9" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>amsurber@contoso.com</v>
+      </c>
+      <c r="AW9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX9" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX9" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>amsurber@contoso.com</v>
       </c>
-      <c r="AY9" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY9" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:amsurber@contoso.com</v>
       </c>
-      <c r="AZ9" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ9" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:amsurber@contoso.com;SIP:amsurber@contoso.com</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="10">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <v>675645</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="12">
         <v>474747</v>
       </c>
-      <c r="F10" s="2" t="str">
+      <c r="F10" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=drobinson,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="24" t="str">
-        <f>TEXT(D10,"0000000")</f>
+      <c r="N10" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0675645</v>
       </c>
-      <c r="O10" t="str">
-        <f t="shared" si="1"/>
+      <c r="O10" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Robinson, Lori</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="R10" s="11" t="s">
+      <c r="R10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y10" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y10" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>drobinson@contoso.com</v>
       </c>
-      <c r="Z10" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z10" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>drobinson</v>
       </c>
-      <c r="AB10" s="2" t="s">
+      <c r="AB10" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AC10" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AD10" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="11">
         <v>10005</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AF10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AH10" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AI10" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AJ10" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK10" s="17">
+      <c r="AK10" s="15">
         <v>23452</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AL10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ10" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>drobinson@contoso.com</v>
-      </c>
-      <c r="AR10" s="21"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" t="str">
-        <f>IF(ISERROR(VLOOKUP(D10,JournalArray2,5,FALSE)),"",VLOOKUP(D10,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU10" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV10" s="6" t="str">
+      <c r="AQ10" s="13" t="str">
         <f t="shared" si="4"/>
         <v>drobinson@contoso.com</v>
       </c>
-      <c r="AW10" s="2" t="s">
+      <c r="AS10" s="17"/>
+      <c r="AT10" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU10" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV10" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>drobinson@contoso.com</v>
+      </c>
+      <c r="AW10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX10" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX10" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>drobinson@contoso.com</v>
       </c>
-      <c r="AY10" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY10" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:drobinson@contoso.com</v>
       </c>
-      <c r="AZ10" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ10" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:drobinson@contoso.com;SIP:drobinson@contoso.com</v>
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="10">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>566778</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="12">
         <v>474747</v>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="F11" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=cjohnson5,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="24" t="str">
-        <f>TEXT(D11,"0000000")</f>
+      <c r="N11" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0566778</v>
       </c>
-      <c r="O11" t="str">
-        <f t="shared" si="1"/>
+      <c r="O11" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Johnson, Mary</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="R11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y11" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y11" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>cjohnson5@contoso.com</v>
       </c>
-      <c r="Z11" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z11" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>cjohnson5</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AB11" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AC11" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AD11" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="11">
         <v>30044</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AF11" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AH11" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AI11" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AJ11" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK11" s="17">
+      <c r="AK11" s="15">
         <v>23452</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AL11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ11" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>cjohnson5@contoso.com</v>
-      </c>
-      <c r="AS11" s="1"/>
-      <c r="AT11" t="str">
-        <f>IF(ISERROR(VLOOKUP(D11,JournalArray2,5,FALSE)),"",VLOOKUP(D11,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU11" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV11" s="6" t="str">
+      <c r="AQ11" s="13" t="str">
         <f t="shared" si="4"/>
         <v>cjohnson5@contoso.com</v>
       </c>
-      <c r="AW11" s="2" t="s">
+      <c r="AS11" s="17"/>
+      <c r="AT11" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU11" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV11" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>cjohnson5@contoso.com</v>
+      </c>
+      <c r="AW11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX11" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX11" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>cjohnson5@contoso.com</v>
       </c>
-      <c r="AY11" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY11" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:cjohnson5@contoso.com</v>
       </c>
-      <c r="AZ11" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ11" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:cjohnson5@contoso.com;SIP:cjohnson5@contoso.com</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="10">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <v>899012</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="12">
         <v>474747</v>
       </c>
-      <c r="F12" s="2" t="str">
+      <c r="F12" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=pwalter,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="24" t="str">
-        <f>TEXT(D12,"0000000")</f>
+      <c r="N12" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0899012</v>
       </c>
-      <c r="O12" t="str">
-        <f t="shared" si="1"/>
+      <c r="O12" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Walker, Mark</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="R12" s="11" t="s">
+      <c r="R12" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y12" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y12" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>pwalter@contoso.com</v>
       </c>
-      <c r="Z12" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z12" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>pwalter</v>
       </c>
-      <c r="AB12" s="2" t="s">
+      <c r="AB12" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AC12" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD12" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="11">
         <v>30044</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AF12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AH12" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AI12" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AJ12" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK12" s="17">
+      <c r="AK12" s="15">
         <v>23452</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AL12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ12" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>pwalter@contoso.com</v>
-      </c>
-      <c r="AR12" s="21"/>
-      <c r="AS12" s="1"/>
-      <c r="AT12" t="str">
-        <f>IF(ISERROR(VLOOKUP(D12,JournalArray2,5,FALSE)),"",VLOOKUP(D12,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU12" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV12" s="6" t="str">
+      <c r="AQ12" s="13" t="str">
         <f t="shared" si="4"/>
         <v>pwalter@contoso.com</v>
       </c>
-      <c r="AW12" s="2" t="s">
+      <c r="AS12" s="17"/>
+      <c r="AT12" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU12" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV12" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>pwalter@contoso.com</v>
+      </c>
+      <c r="AW12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX12" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX12" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>pwalter@contoso.com</v>
       </c>
-      <c r="AY12" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY12" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:pwalter@contoso.com</v>
       </c>
-      <c r="AZ12" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ12" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:pwalter@contoso.com;SIP:pwalter@contoso.com</v>
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="10">
         <v>0</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>101918</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="12">
         <v>566778</v>
       </c>
-      <c r="F13" s="2" t="str">
+      <c r="F13" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=pdloughy,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="N13" s="24" t="str">
-        <f>TEXT(D13,"0000000")</f>
+      <c r="N13" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0101918</v>
       </c>
-      <c r="O13" t="str">
-        <f t="shared" si="1"/>
+      <c r="O13" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Doughty, Manny</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="R13" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y13" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y13" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>pdloughy@contoso.com</v>
       </c>
-      <c r="Z13" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z13" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>pdloughy</v>
       </c>
-      <c r="AB13" s="2" t="s">
+      <c r="AB13" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AC13" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AD13" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="11">
         <v>30044</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AH13" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AI13" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AJ13" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK13" s="17">
+      <c r="AK13" s="15">
         <v>23452</v>
       </c>
-      <c r="AL13" t="s">
+      <c r="AL13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ13" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>pdloughy@contoso.com</v>
-      </c>
-      <c r="AR13" s="21"/>
-      <c r="AS13" s="1"/>
-      <c r="AT13" t="str">
-        <f>IF(ISERROR(VLOOKUP(D13,JournalArray2,5,FALSE)),"",VLOOKUP(D13,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU13" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV13" s="6" t="str">
+      <c r="AQ13" s="13" t="str">
         <f t="shared" si="4"/>
         <v>pdloughy@contoso.com</v>
       </c>
-      <c r="AW13" s="2" t="s">
+      <c r="AS13" s="17"/>
+      <c r="AT13" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU13" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV13" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>pdloughy@contoso.com</v>
+      </c>
+      <c r="AW13" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX13" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX13" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>pdloughy@contoso.com</v>
       </c>
-      <c r="AY13" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY13" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:pdloughy@contoso.com</v>
       </c>
-      <c r="AZ13" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ13" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:pdloughy@contoso.com;SIP:pdloughy@contoso.com</v>
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="10">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="11">
         <v>292827</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="12">
         <v>566778</v>
       </c>
-      <c r="F14" s="2" t="str">
+      <c r="F14" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=wdegroat,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="2" t="str">
+      <c r="I14" s="11" t="str">
         <f>H14</f>
         <v>wdegroat</v>
       </c>
-      <c r="J14" s="2" t="str">
+      <c r="J14" s="11" t="str">
         <f>H14</f>
         <v>wdegroat</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="N14" s="24" t="str">
-        <f>TEXT(D14,"0000000")</f>
+      <c r="N14" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0292827</v>
       </c>
-      <c r="O14" t="str">
-        <f t="shared" si="1"/>
+      <c r="O14" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Simmons, Bill</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="S14" s="14"/>
-      <c r="U14" t="s">
+      <c r="U14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y14" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y14" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>wdegroat@contoso.com</v>
       </c>
-      <c r="Z14" s="14" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z14" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>wdegroat</v>
       </c>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="2" t="s">
+      <c r="AB14" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AC14" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="11">
         <v>30044</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AF14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AH14" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AI14" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AJ14" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK14" s="17">
+      <c r="AK14" s="15">
         <v>23452</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AL14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AP14" s="2"/>
-      <c r="AQ14" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>wdegroat@contoso.com</v>
-      </c>
-      <c r="AR14" s="21"/>
-      <c r="AS14" s="5"/>
-      <c r="AT14" t="str">
-        <f>IF(ISERROR(VLOOKUP(D14,JournalArray2,5,FALSE)),"",VLOOKUP(D14,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU14" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV14" s="6" t="str">
+      <c r="AQ14" s="13" t="str">
         <f t="shared" si="4"/>
         <v>wdegroat@contoso.com</v>
       </c>
-      <c r="AW14" s="2" t="s">
+      <c r="AS14" s="17"/>
+      <c r="AT14" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU14" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV14" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>wdegroat@contoso.com</v>
+      </c>
+      <c r="AW14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX14" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX14" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>wdegroat@contoso.com</v>
       </c>
-      <c r="AY14" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY14" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:wdegroat@contoso.com</v>
       </c>
-      <c r="AZ14" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ14" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:wdegroat@contoso.com;SIP:wdegroat@contoso.com</v>
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="10">
         <v>0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="11">
         <v>383736</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="12">
         <v>566778</v>
       </c>
-      <c r="F15" s="2" t="str">
+      <c r="F15" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=tscarfone,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="N15" s="24" t="str">
-        <f>TEXT(D15,"0000000")</f>
+      <c r="N15" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0383736</v>
       </c>
-      <c r="O15" t="str">
-        <f t="shared" si="1"/>
+      <c r="O15" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Thompson, Bob</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="R15" s="11" t="s">
+      <c r="R15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y15" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y15" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>tscarfone@contoso.com</v>
       </c>
-      <c r="Z15" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z15" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>tscarfone</v>
       </c>
-      <c r="AB15" s="2" t="s">
+      <c r="AB15" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AC15" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AD15" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="AE15">
+      <c r="AE15" s="11">
         <v>20004</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AF15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AH15" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AI15" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AJ15" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK15" s="17">
+      <c r="AK15" s="15">
         <v>23452</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AL15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ15" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>tscarfone@contoso.com</v>
-      </c>
-      <c r="AR15" s="21"/>
-      <c r="AS15" s="1"/>
-      <c r="AT15" t="str">
-        <f>IF(ISERROR(VLOOKUP(D15,JournalArray2,5,FALSE)),"",VLOOKUP(D15,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU15" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV15" s="6" t="str">
+      <c r="AQ15" s="13" t="str">
         <f t="shared" si="4"/>
         <v>tscarfone@contoso.com</v>
       </c>
-      <c r="AW15" s="2" t="s">
+      <c r="AS15" s="17"/>
+      <c r="AT15" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU15" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV15" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>tscarfone@contoso.com</v>
+      </c>
+      <c r="AW15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX15" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX15" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>tscarfone@contoso.com</v>
       </c>
-      <c r="AY15" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY15" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:tscarfone@contoso.com</v>
       </c>
-      <c r="AZ15" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ15" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:tscarfone@contoso.com;SIP:tscarfone@contoso.com</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="10">
         <v>0</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="11">
         <v>484746</v>
       </c>
-      <c r="F16" s="2" t="str">
+      <c r="F16" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=mvillarreal,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="N16" s="24" t="str">
-        <f>TEXT(D16,"0000000")</f>
+      <c r="N16" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0484746</v>
       </c>
-      <c r="O16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O16" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Su, Barbara</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U16" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y16" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y16" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>mvillarreal@contoso.com</v>
       </c>
-      <c r="Z16" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z16" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>mvillarreal</v>
       </c>
-      <c r="AB16" s="2" t="s">
+      <c r="AB16" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AC16" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AD16" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="AE16">
+      <c r="AE16" s="11">
         <v>20004</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AF16" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AH16" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AI16" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AJ16" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK16" s="17">
+      <c r="AK16" s="15">
         <v>23452</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="AL16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ16" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>mvillarreal@contoso.com</v>
-      </c>
-      <c r="AR16" s="21"/>
-      <c r="AS16" s="1"/>
-      <c r="AT16" t="str">
-        <f>IF(ISERROR(VLOOKUP(D16,JournalArray2,5,FALSE)),"",VLOOKUP(D16,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU16" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV16" s="6" t="str">
+      <c r="AQ16" s="13" t="str">
         <f t="shared" si="4"/>
         <v>mvillarreal@contoso.com</v>
       </c>
-      <c r="AW16" s="2" t="s">
+      <c r="AS16" s="17"/>
+      <c r="AT16" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU16" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV16" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>mvillarreal@contoso.com</v>
+      </c>
+      <c r="AW16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX16" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX16" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>mvillarreal@contoso.com</v>
       </c>
-      <c r="AY16" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY16" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:mvillarreal@contoso.com</v>
       </c>
-      <c r="AZ16" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ16" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:mvillarreal@contoso.com;SIP:mvillarreal@contoso.com</v>
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="10">
         <v>0</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="11">
         <v>595058</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="12">
         <v>484746</v>
       </c>
-      <c r="F17" s="2" t="str">
+      <c r="F17" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=ksweeney1,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="24" t="str">
-        <f>TEXT(D17,"0000000")</f>
+      <c r="N17" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0595058</v>
       </c>
-      <c r="O17" t="str">
-        <f t="shared" si="1"/>
+      <c r="O17" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Charles, David</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="R17" s="11" t="s">
+      <c r="R17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y17" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y17" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>ksweeney1@contoso.com</v>
       </c>
-      <c r="Z17" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z17" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>ksweeney1</v>
       </c>
-      <c r="AB17" s="2" t="s">
+      <c r="AB17" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AC17" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AD17" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="AE17">
+      <c r="AE17" s="11">
         <v>20005</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AF17" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AH17" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AI17" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AJ17" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK17" s="17">
+      <c r="AK17" s="15">
         <v>23452</v>
       </c>
-      <c r="AL17" t="s">
+      <c r="AL17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ17" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>ksweeney1@contoso.com</v>
-      </c>
-      <c r="AR17" s="21"/>
-      <c r="AS17" s="1"/>
-      <c r="AT17" t="str">
-        <f>IF(ISERROR(VLOOKUP(D17,JournalArray2,5,FALSE)),"",VLOOKUP(D17,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU17" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV17" s="6" t="str">
+      <c r="AQ17" s="13" t="str">
         <f t="shared" si="4"/>
         <v>ksweeney1@contoso.com</v>
       </c>
-      <c r="AW17" s="2" t="s">
+      <c r="AS17" s="17"/>
+      <c r="AT17" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU17" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV17" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>ksweeney1@contoso.com</v>
+      </c>
+      <c r="AW17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX17" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX17" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>ksweeney1@contoso.com</v>
       </c>
-      <c r="AY17" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY17" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:ksweeney1@contoso.com</v>
       </c>
-      <c r="AZ17" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ17" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:ksweeney1@contoso.com;SIP:ksweeney1@contoso.com</v>
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="10">
         <v>0</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="11">
         <v>696867</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="12">
         <v>484746</v>
       </c>
-      <c r="F18" s="2" t="str">
+      <c r="F18" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=irevuelta,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="N18" s="24" t="str">
-        <f>TEXT(D18,"0000000")</f>
+      <c r="N18" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0696867</v>
       </c>
-      <c r="O18" t="str">
-        <f t="shared" si="1"/>
+      <c r="O18" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Roberts, Donald</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="R18" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y18" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y18" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>irevuelta@contoso.com</v>
       </c>
-      <c r="Z18" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z18" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>irevuelta</v>
       </c>
-      <c r="AB18" s="2" t="s">
+      <c r="AB18" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AC18" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AD18" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="11">
         <v>20005</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AF18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AG18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AH18" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AI18" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AJ18" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK18" s="17">
+      <c r="AK18" s="15">
         <v>23452</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AL18" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ18" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>irevuelta@contoso.com</v>
-      </c>
-      <c r="AR18" s="21"/>
-      <c r="AS18" s="1"/>
-      <c r="AT18" t="str">
-        <f>IF(ISERROR(VLOOKUP(D18,JournalArray2,5,FALSE)),"",VLOOKUP(D18,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU18" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV18" s="6" t="str">
+      <c r="AQ18" s="13" t="str">
         <f t="shared" si="4"/>
         <v>irevuelta@contoso.com</v>
       </c>
-      <c r="AW18" s="2" t="s">
+      <c r="AS18" s="17"/>
+      <c r="AT18" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU18" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV18" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>irevuelta@contoso.com</v>
+      </c>
+      <c r="AW18" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX18" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX18" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>irevuelta@contoso.com</v>
       </c>
-      <c r="AY18" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY18" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:irevuelta@contoso.com</v>
       </c>
-      <c r="AZ18" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ18" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:irevuelta@contoso.com;SIP:irevuelta@contoso.com</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="10">
         <v>0</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="11">
         <v>131415</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="12">
         <v>484746</v>
       </c>
-      <c r="F19" s="2" t="str">
+      <c r="F19" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=csoto,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="N19" s="24" t="str">
-        <f>TEXT(D19,"0000000")</f>
+      <c r="N19" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0131415</v>
       </c>
-      <c r="O19" t="str">
-        <f t="shared" si="1"/>
+      <c r="O19" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Valenza, Denise</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q19" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="R19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U19" t="s">
+      <c r="U19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y19" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y19" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>csoto@contoso.com</v>
       </c>
-      <c r="Z19" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z19" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>csoto</v>
       </c>
-      <c r="AB19" s="2" t="s">
+      <c r="AB19" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AC19" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AD19" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="11">
         <v>20006</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AF19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AG19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AH19" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AI19" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ19" t="s">
+      <c r="AJ19" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK19" s="17">
+      <c r="AK19" s="15">
         <v>23452</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AL19" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ19" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>csoto@contoso.com</v>
-      </c>
-      <c r="AR19" s="21"/>
-      <c r="AS19" s="1"/>
-      <c r="AT19" t="str">
-        <f>IF(ISERROR(VLOOKUP(D19,JournalArray2,5,FALSE)),"",VLOOKUP(D19,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU19" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV19" s="6" t="str">
+      <c r="AQ19" s="13" t="str">
         <f t="shared" si="4"/>
         <v>csoto@contoso.com</v>
       </c>
-      <c r="AW19" s="2" t="s">
+      <c r="AS19" s="17"/>
+      <c r="AT19" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU19" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV19" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>csoto@contoso.com</v>
+      </c>
+      <c r="AW19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX19" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX19" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>csoto@contoso.com</v>
       </c>
-      <c r="AY19" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY19" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:csoto@contoso.com</v>
       </c>
-      <c r="AZ19" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ19" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:csoto@contoso.com;SIP:csoto@contoso.com</v>
       </c>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20" s="10">
         <v>0</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="11">
         <v>262728</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="12">
         <v>484746</v>
       </c>
-      <c r="F20" s="2" t="str">
+      <c r="F20" s="11" t="str">
         <f t="shared" si="0"/>
         <v>CN=dstevenson,OU=Users,OU=Corp,DC=contoso,DC=com</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="24" t="str">
-        <f>TEXT(D20,"0000000")</f>
+      <c r="N20" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>0262728</v>
       </c>
-      <c r="O20" t="str">
-        <f t="shared" si="1"/>
+      <c r="O20" s="11" t="str">
+        <f t="shared" si="2"/>
         <v>Stevenson, Allen</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q20" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="R20" s="11" t="s">
+      <c r="R20" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U20" t="s">
+      <c r="U20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Y20" s="11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Y20" s="13" t="str">
+        <f t="shared" si="10"/>
         <v>dstevenson@contoso.com</v>
       </c>
-      <c r="Z20" s="13" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z20" s="10" t="str">
+        <f t="shared" si="3"/>
         <v>dstevenson</v>
       </c>
-      <c r="AB20" s="2" t="s">
+      <c r="AB20" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AC20" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AD20" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="AE20">
+      <c r="AE20" s="11">
         <v>20006</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AF20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AG20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AH20" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AI20" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="AJ20" t="s">
+      <c r="AJ20" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="AK20" s="17">
+      <c r="AK20" s="15">
         <v>23452</v>
       </c>
-      <c r="AL20" t="s">
+      <c r="AL20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AQ20" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>dstevenson@contoso.com</v>
-      </c>
-      <c r="AR20" s="21"/>
-      <c r="AS20" s="1"/>
-      <c r="AT20" t="str">
-        <f>IF(ISERROR(VLOOKUP(D20,JournalArray2,5,FALSE)),"",VLOOKUP(D20,JournalArray2,5,FALSE))</f>
-        <v/>
-      </c>
-      <c r="AU20" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AV20" s="6" t="str">
+      <c r="AQ20" s="13" t="str">
         <f t="shared" si="4"/>
         <v>dstevenson@contoso.com</v>
       </c>
-      <c r="AW20" s="2" t="s">
+      <c r="AS20" s="17"/>
+      <c r="AT20" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AU20" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AV20" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>dstevenson@contoso.com</v>
+      </c>
+      <c r="AW20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AX20" s="6" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX20" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>dstevenson@contoso.com</v>
       </c>
-      <c r="AY20" t="str">
-        <f t="shared" si="6"/>
+      <c r="AY20" s="11" t="str">
+        <f t="shared" si="8"/>
         <v>SIP:dstevenson@contoso.com</v>
       </c>
-      <c r="AZ20" s="2" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ20" s="11" t="str">
+        <f t="shared" si="9"/>
         <v>SMTP:dstevenson@contoso.com;SIP:dstevenson@contoso.com</v>
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AK21"/>
-      <c r="AS21" s="1"/>
-      <c r="AV21" s="6"/>
-      <c r="AW21" s="2"/>
-      <c r="AX21" s="6"/>
-      <c r="AZ21" s="2"/>
+      <c r="AK21" s="11"/>
+      <c r="AS21" s="17"/>
+      <c r="AV21" s="13"/>
+      <c r="AX21" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AZ21"/>
+  <autoFilter ref="A1:AZ21" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
@@ -5067,7 +5037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5081,47 +5051,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2">
         <v>123123</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3">
         <v>474747</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4">
         <v>484746</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5">
         <v>566778</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C5">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B5">
@@ -5133,6 +5103,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <RIMStatus xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">New Metlife Document</RIMStatus>
+    <RIMInDispositionReview xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</RIMInDispositionReview>
+    <GIPClassCodeTaxHTField0 xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </GIPClassCodeTaxHTField0>
+    <RIMNamedEvent xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">id-1;#RIMBlank</RIMNamedEvent>
+    <RIMCountryTaxHTField0 xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </RIMCountryTaxHTField0>
+    <Area xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf" xsi:nil="true"/>
+    <Hidden_x003f_ xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</Hidden_x003f_>
+    <DocType xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf" xsi:nil="true"/>
+    <TaxCatchAll xmlns="32f2367a-313f-43c9-b9ab-26948e9e8ba4"/>
+    <GIPEventDate xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf" xsi:nil="true"/>
+    <RIMIsInRecordsCenter xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</RIMIsInRecordsCenter>
+    <RIMIsSuperseded xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</RIMIsSuperseded>
+    <RIMFarmId xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">d631f93c-4dc4-4574-b44b-b8deb029919d</RIMFarmId>
+    <_dlc_DocId xmlns="32f2367a-313f-43c9-b9ab-26948e9e8ba4">ML551551-34-784</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="32f2367a-313f-43c9-b9ab-26948e9e8ba4">
+      <Url>https://team.amer.mymetlife.com/teams/EIAOutboundProjectMgmt/jtmp/usr/_layouts/DocIdRedir.aspx?ID=ML551551-34-784</Url>
+      <Description>ML551551-34-784</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5248,45 +5256,39 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:Policy xmlns:p="office.server.policy" id="" local="true">
+  <p:Name>MetLife Document</p:Name>
+  <p:Description/>
+  <p:Statement/>
+  <p:PolicyItems>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration" staticId="0x0101000728167CD9C94899925BA69C4AF6743E|1070707530" UniqueId="c963c7f9-86ab-47ed-84d2-46963c30ff53">
+      <p:Name>Retention</p:Name>
+      <p:Description>Automatic scheduling of content for processing, and performing a retention action on content that has reached its due date.</p:Description>
+      <p:CustomData>
+        <Schedules nextStageId="2">
+          <Schedule type="Default">
+            <stages>
+              <data>
+                <formula id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Formula.BuiltIn">
+                  <number>12</number>
+                  <property>_vti_ItemDeclaredRecord</property>
+                  <propertyId>f9a44731-84eb-43a4-9973-cd2953ad8646</propertyId>
+                  <period>months</period>
+                </formula>
+                <action type="action" id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Action.DeletePreviousVersions"/>
+              </data>
+            </stages>
+          </Schedule>
+        </Schedules>
+      </p:CustomData>
+    </p:PolicyItem>
+  </p:PolicyItems>
+</p:Policy>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <RIMStatus xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">New Metlife Document</RIMStatus>
-    <RIMInDispositionReview xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</RIMInDispositionReview>
-    <GIPClassCodeTaxHTField0 xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </GIPClassCodeTaxHTField0>
-    <RIMNamedEvent xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">id-1;#RIMBlank</RIMNamedEvent>
-    <RIMCountryTaxHTField0 xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </RIMCountryTaxHTField0>
-    <Area xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf" xsi:nil="true"/>
-    <Hidden_x003f_ xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</Hidden_x003f_>
-    <DocType xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf" xsi:nil="true"/>
-    <TaxCatchAll xmlns="32f2367a-313f-43c9-b9ab-26948e9e8ba4"/>
-    <GIPEventDate xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf" xsi:nil="true"/>
-    <RIMIsInRecordsCenter xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</RIMIsInRecordsCenter>
-    <RIMIsSuperseded xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">false</RIMIsSuperseded>
-    <RIMFarmId xmlns="a922f92c-ebd9-4408-ae39-b4e66478dbaf">d631f93c-4dc4-4574-b44b-b8deb029919d</RIMFarmId>
-    <_dlc_DocId xmlns="32f2367a-313f-43c9-b9ab-26948e9e8ba4">ML551551-34-784</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="32f2367a-313f-43c9-b9ab-26948e9e8ba4">
-      <Url>https://team.amer.mymetlife.com/teams/EIAOutboundProjectMgmt/jtmp/usr/_layouts/DocIdRedir.aspx?ID=ML551551-34-784</Url>
-      <Description>ML551551-34-784</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="MetLife Document" ma:contentTypeID="0x0101000728167CD9C94899925BA69C4AF6743E0039DF1EBF3502D6429F2214A003788B1C" ma:contentTypeVersion="20" ma:contentTypeDescription="MetLife Document Content Type" ma:contentTypeScope="" ma:versionID="9ac2f7dcdb00b2695b2f264525a9daf5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="32f2367a-313f-43c9-b9ab-26948e9e8ba4" xmlns:ns3="a922f92c-ebd9-4408-ae39-b4e66478dbaf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="adf6a2260baecb662824601b6d581759" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5635,55 +5637,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<p:Policy xmlns:p="office.server.policy" id="" local="true">
-  <p:Name>MetLife Document</p:Name>
-  <p:Description/>
-  <p:Statement/>
-  <p:PolicyItems>
-    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration" staticId="0x0101000728167CD9C94899925BA69C4AF6743E|1070707530" UniqueId="c963c7f9-86ab-47ed-84d2-46963c30ff53">
-      <p:Name>Retention</p:Name>
-      <p:Description>Automatic scheduling of content for processing, and performing a retention action on content that has reached its due date.</p:Description>
-      <p:CustomData>
-        <Schedules nextStageId="2">
-          <Schedule type="Default">
-            <stages>
-              <data>
-                <formula id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Formula.BuiltIn">
-                  <number>12</number>
-                  <property>_vti_ItemDeclaredRecord</property>
-                  <propertyId>f9a44731-84eb-43a4-9973-cd2953ad8646</propertyId>
-                  <period>months</period>
-                </formula>
-                <action type="action" id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Action.DeletePreviousVersions"/>
-              </data>
-            </stages>
-          </Schedule>
-        </Schedules>
-      </p:CustomData>
-    </p:PolicyItem>
-  </p:PolicyItems>
-</p:Policy>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81826189-B050-4C00-8975-67CE7489426D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3FA5E59-C381-46C2-9B09-39AD21E93264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{187A00F1-70DB-4C9E-A147-9E48EC579204}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5701,7 +5655,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3FA5E59-C381-46C2-9B09-39AD21E93264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81826189-B050-4C00-8975-67CE7489426D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C3DE198-7C29-4450-8E66-4A5F12118BB0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="office.server.policy"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA7AD069-84D3-4B71-B53F-9E30F055AD03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5719,12 +5697,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C3DE198-7C29-4450-8E66-4A5F12118BB0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="office.server.policy"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>